<commit_message>
fix jieba dict bug
</commit_message>
<xml_diff>
--- a/preprocess/数据处理-操作记录.xlsx
+++ b/preprocess/数据处理-操作记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnymarkliu/Projects/DeepLearning/multi_passages_mrc/preprocess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC36404F-3A55-594E-9A4F-913BB121911D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0461F459-A15A-4440-9ED4-6D9A1D3A83AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17040" xr2:uid="{039241F0-9446-3D4E-BBDF-ACEB2710A2CB}"/>
   </bookViews>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F698B644-3737-5048-8E44-D93A0A367B3D}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>